<commit_message>
new first pytestClass: queryQy.py
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myapp\DemoTest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myapp\pyTest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81185130-E630-4BB6-BB88-6C98D776D18D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B351B8BB-E6FB-4AC6-9FF6-022C8F48C374}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="3360" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mtPossession" sheetId="1" r:id="rId1"/>
     <sheet name="juhe" sheetId="2" r:id="rId2"/>
     <sheet name="register" sheetId="3" r:id="rId3"/>
+    <sheet name="JD查询企业信息" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>test_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +87,105 @@
   </si>
   <si>
     <t>{"validateKey": “”, "type": "1", "telNum": tel_num,"autoCode": "0000", "businessType": 1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_description</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enterpriseName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssoId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>platform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qyd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1445898791152850915</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>参数错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50004</t>
+  </si>
+  <si>
+    <t>50007</t>
+  </si>
+  <si>
+    <t>50008</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>数据库操作错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询服务已关闭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用第三方其他错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JD业务失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长沙市天心区祝博士教育信息咨询服务部</t>
+  </si>
+  <si>
+    <t>长沙市天心区祝博士教育信息咨询服务部</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -93,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +207,41 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -123,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,20 +266,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 3" xfId="1" xr:uid="{3642DA88-6F18-4499-8AC4-358AAA173E22}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -523,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7611B01E-3CBB-44AE-99F7-E2C75C2CD00D}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -580,4 +746,236 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D41525-F88C-48A4-BC30-B64798EAA0B9}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.375" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>